<commit_message>
Deploying to main from @ pedalboard/pedalboard-display@f8f95626dab1886cdfae880860ee8407afd30411 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Generic/pedalboard-display-bom.xlsx
+++ b/latest/BoM/Generic/pedalboard-display-bom.xlsx
@@ -8,19 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="BoM" sheetId="1" r:id="rId1"/>
-    <sheet name="DNF" sheetId="2" r:id="rId2"/>
-    <sheet name="Colors" sheetId="3" r:id="rId3"/>
+    <sheet name="Colors" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">BoM!$9:$9</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">DNF!$9:$9</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="70">
   <si>
     <t>Row</t>
   </si>
@@ -55,13 +53,13 @@
     <t>1</t>
   </si>
   <si>
-    <t>Unpolarized capacitor, small symbol</t>
+    <t/>
   </si>
   <si>
     <t>C</t>
   </si>
   <si>
-    <t>C1 C2 C3 C4 C5 C6 C7 C8 C9 C10 C11 C12 C13 C14 C15 C16 C17 C18 C19 C20 C21 C22 C23 C24 C25 C26 C27 C28 C29 C30 C31 C32 C33 C34 C35 C36 C37 C38 C39 C40 C41 C42 C43 C44 C45 C46 C47 C48 C49 C50 C51 C52 C53 C54 C55 C56 C57 C58 C59 C60 C61 C62 C63 C64 C65 C66 C67 C68 C69 C70 C71 C72 C73 C74 C75 C76 C77 C78 C79 C80 C81 C82 C83 C84 C85 C86 C87 C88 C89 C90 C91 C92 C93 C94 C95 C96 C97 C98 C99 C100 C103 C104</t>
+    <t>C1 C2 C3 C4 C5 C6 C7 C8 C9 C10 C11 C12 C13 C14 C15 C16 C17 C18 C19 C20 C21 C22 C23 C24 C25 C26 C27 C28 C29 C30 C31 C32 C33 C34 C35 C36 C37 C38 C39 C40 C41 C42 C43 C44 C45 C46 C47 C48 C49 C50 C51 C52 C53 C54 C55 C56 C57 C58 C59 C60 C61 C62 C63 C64 C65 C66 C67 C68 C69 C70 C71 C72 C73 C74 C75 C76 C77 C78 C79 C80 C81 C82 C83 C84 C85 C86 C87 C88 C89 C90 C91 C92 C93 C94 C95 C96 C97 C98</t>
   </si>
   <si>
     <t>1uF</t>
@@ -70,7 +68,7 @@
     <t>C_0402_1005Metric</t>
   </si>
   <si>
-    <t>102</t>
+    <t>98</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -85,145 +83,85 @@
     <t>2</t>
   </si>
   <si>
-    <t>C_Small</t>
-  </si>
-  <si>
-    <t>C101 C102 C105 C106</t>
-  </si>
-  <si>
-    <t>10uF</t>
-  </si>
-  <si>
-    <t/>
+    <t>SK6812</t>
+  </si>
+  <si>
+    <t>D1 D2 D3 D4 D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D31 D32 D33 D34 D35 D36 D37 D38 D39 D40 D41 D42 D43 D44 D45 D46 D47 D48 D49 D50 D51 D52 D53 D54 D55 D56 D57 D58 D59 D60 D61 D62 D63 D64 D65 D66 D67 D68 D69 D70 D71 D72 D73 D74 D75 D76 D77 D78 D79 D80 D81 D82 D83 D84 D85 D86 D87 D88 D89 D90 D91 D92 D93 D94 D95 D96 D97 D98</t>
+  </si>
+  <si>
+    <t>SK6812_EC15</t>
+  </si>
+  <si>
+    <t>LED_SK6812_EC15_1.5x1.5mm</t>
+  </si>
+  <si>
+    <t>https://mm.digikey.com/Volume0/opasdata/d220001/medias/docus/2384/CL05A105KP5NNN_Specsheet%20(1).pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/en/products/detail/adafruit-industries-llc/4492/11569136</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Conn_01x03_Pin</t>
+  </si>
+  <si>
+    <t>J1 J2</t>
+  </si>
+  <si>
+    <t>JST_PH_B3B-PH-SM4-TB_1x03-1MP_P2.00mm_Vertical</t>
+  </si>
+  <si>
+    <t>~</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>~</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>SK6812</t>
-  </si>
-  <si>
-    <t>D1 D2 D3 D4 D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D31 D32 D33 D34 D35 D36 D37 D38 D39 D40 D41 D42 D43 D44 D45 D46 D47 D48 D49 D50 D51 D52 D53 D54 D55 D56 D57 D58 D59 D60 D61 D62 D63 D64 D65 D66 D67 D68 D69 D70 D71 D72 D73 D74 D75 D76 D77 D78 D79 D80 D81 D82 D83 D84 D85 D86 D87 D88 D89 D90 D91 D92 D93 D94 D95 D96 D97 D98</t>
-  </si>
-  <si>
-    <t>SK6812_EC15</t>
-  </si>
-  <si>
-    <t>LED_SK6812_EC15_1.5x1.5mm</t>
-  </si>
-  <si>
-    <t>98</t>
-  </si>
-  <si>
-    <t>https://mm.digikey.com/Volume0/opasdata/d220001/medias/docus/2384/CL05A105KP5NNN_Specsheet%20(1).pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/en/products/detail/adafruit-industries-llc/4492/11569136</t>
-  </si>
-  <si>
-    <t>OLED display 128x64</t>
-  </si>
-  <si>
-    <t>OLED-128O064D</t>
-  </si>
-  <si>
-    <t>DS1 DS2</t>
-  </si>
-  <si>
-    <t>https://www.vishay.com/docs/37902/oled128o064dbpp3n00000.pdf</t>
+    <t>Generic connector, single row, 01x04, script generated</t>
+  </si>
+  <si>
+    <t>Conn_01x04_Pin</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>OLED</t>
+  </si>
+  <si>
+    <t>JST_PH_B4B-PH-SM4-TB_1x04-1MP_P2.00mm_Vertical</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t>Conn_01x03_Pin</t>
-  </si>
-  <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>JST_PH_B3B-PH-SM4-TB_1x03-1MP_P2.00mm_Vertical</t>
+    <t>R</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>330</t>
+  </si>
+  <si>
+    <t>R_0402_1005Metric</t>
+  </si>
+  <si>
+    <t>https://www.passivecomponent.com/wp-content/uploads/chipR/ASC_WR.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/en/products/detail/walsin-technology-corporation/WR04X3300FTL/13239224</t>
   </si>
   <si>
     <t>6</t>
   </si>
   <si>
-    <t>Generic connector, single row, 01x04, script generated</t>
-  </si>
-  <si>
-    <t>Conn_01x04_Pin</t>
-  </si>
-  <si>
-    <t>J3</t>
-  </si>
-  <si>
-    <t>OLED STEMMA</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>330</t>
-  </si>
-  <si>
-    <t>R_0402_1005Metric</t>
-  </si>
-  <si>
-    <t>https://www.passivecomponent.com/wp-content/uploads/chipR/ASC_WR.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/en/products/detail/walsin-technology-corporation/WR04X3300FTL/13239224</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>10K</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>R3 R5</t>
-  </si>
-  <si>
-    <t>390K</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>push-pull, active-high, 200mS reset delay, 2.93V threshold voltage, SOT-23</t>
-  </si>
-  <si>
-    <t>TLV810EA29DBZ</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>SOT-23</t>
-  </si>
-  <si>
-    <t>https://www.ti.com/lit/ds/symlink/tlv803e.pdf</t>
+    <t>U1 U2</t>
+  </si>
+  <si>
+    <t>OLED_128x128</t>
   </si>
   <si>
     <t>KiBot Bill of Materials</t>
@@ -250,7 +188,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2024-10-04</t>
+    <t>2024-10-05</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -265,28 +203,16 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>216 (205 SMD/ 0 THT)</t>
+    <t>202 (200 SMD/ 2 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
   </si>
   <si>
-    <t>213 (204 SMD/ 0 THT)</t>
-  </si>
-  <si>
     <t>Number of PCBs:</t>
   </si>
   <si>
     <t>Total Components:</t>
-  </si>
-  <si>
-    <t>J2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (DNF)</t>
-  </si>
-  <si>
-    <t>R6 R7</t>
   </si>
   <si>
     <t>Columns colors</t>
@@ -361,7 +287,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE6F9FF"/>
+        <fgColor rgb="FFFF8080"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -373,13 +299,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFE6F9FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF0FFF4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF0FFFF"/>
+        <fgColor rgb="FFFF8A8A"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -391,13 +323,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF8A8A"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF8080"/>
+        <fgColor rgb="FFF0FFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -473,58 +399,6 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1464384</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>123779</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
-              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="1"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="2378784" cy="1285829"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>16584</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
@@ -850,7 +724,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -860,7 +734,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="60.7109375" customWidth="1"/>
+    <col min="2" max="2" width="59.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="60.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
@@ -873,7 +747,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -885,55 +759,55 @@
     </row>
     <row r="2" spans="1:10">
       <c r="C2" s="2" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="F2" s="3">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="C3" s="2" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="C4" s="2" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="C5" s="2" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -941,16 +815,16 @@
     </row>
     <row r="6" spans="1:10">
       <c r="C6" s="2" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="F6" s="3">
-        <v>213</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1013,48 +887,48 @@
       <c r="I9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:10" ht="105" customHeight="1">
+      <c r="A10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="11" t="s">
         <v>23</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="11" t="s">
+      <c r="J10" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="105" customHeight="1">
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>24</v>
+      <c r="B11" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>28</v>
@@ -1063,71 +937,71 @@
         <v>29</v>
       </c>
       <c r="E11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>31</v>
-      </c>
       <c r="G11" s="5" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="C12" s="11" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="9" t="s">
+      <c r="D12" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="E12" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="F12" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="8" t="s">
+      <c r="G12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="9" t="s">
         <v>17</v>
       </c>
       <c r="I12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" customHeight="1">
+      <c r="A13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J12" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="5" t="s">
+      <c r="B13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="7" t="s">
+      <c r="D13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="E13" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>42</v>
@@ -1138,171 +1012,43 @@
       <c r="H13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>24</v>
+      <c r="I13" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="B14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>46</v>
       </c>
       <c r="E14" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="8" t="s">
+      <c r="G14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I14" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="30" customHeight="1">
-      <c r="A15" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="J17" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="30" customHeight="1">
-      <c r="A18" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I18" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="J18" s="11" t="s">
-        <v>24</v>
+      <c r="I14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1317,217 +1063,6 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1"/>
-    <col min="6" max="6" width="51.7109375" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="32" customHeight="1">
-      <c r="C1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="C2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F2" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="C3" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="C4" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="C5" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="C6" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F6" s="3">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C1:J1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1539,27 +1074,27 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="6" t="s">
-        <v>92</v>
+      <c r="A4" s="8" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="12" t="s">
-        <v>93</v>
+      <c r="A5" s="6" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>